<commit_message>
Adding examples, changing URIs to https
</commit_message>
<xml_diff>
--- a/test_data/sample/CATALOG_sample.xlsx
+++ b/test_data/sample/CATALOG_sample.xlsx
@@ -16,21 +16,6 @@
     <sheet name="Projects" sheetId="11" r:id="rId11"/>
   </sheets>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>None</author>
-  </authors>
-  <commentList>
-    <comment ref="B6" authorId="0">
-      <text>
-        <t>Put the ID of a Person or Organisation here</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,10 +433,10 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>RELATION:Contact</v>
+        <v>RELATION:contactPoint</v>
       </c>
       <c r="B6" t="str">
-        <v>Peter Sefton</v>
+        <v>peter.sefton@uts.edu.au</v>
       </c>
     </row>
     <row r="7">
@@ -513,9 +498,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -666,7 +651,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="People"/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -696,6 +681,9 @@
       <c r="H1" t="str">
         <v>TYPE:</v>
       </c>
+      <c r="I1" t="str">
+        <v>contactPoint&gt;TYPE:ContactPoint&gt;</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -718,6 +706,9 @@
       </c>
       <c r="H2" t="str">
         <v>Person</v>
+      </c>
+      <c r="I2" t="str">
+        <v>ID: peter.sefton@uts.edu.au, contactType: customer service, email: peter.sefton@uts.edu.au, URL: http://orcid.org/0000-0002-3545-944X, name: Contact Peter Sefton</v>
       </c>
     </row>
   </sheetData>
@@ -883,7 +874,7 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Actions"/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -899,18 +890,21 @@
         <v>TYPE:</v>
       </c>
       <c r="D1" t="str">
+        <v>endTime</v>
+      </c>
+      <c r="E1" t="str">
         <v>RELATION:Result</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>RELATION:Object</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>RELATION:Instrument*</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>RELATION:Agent</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>Description</v>
       </c>
     </row>
@@ -925,15 +919,21 @@
         <v>CreateAction</v>
       </c>
       <c r="D2" t="str">
+        <v>2017:06:11T12:56:14+10:00</v>
+      </c>
+      <c r="E2" t="str">
         <v>pics/2017-06-11 12.56.14.jpg</v>
       </c>
       <c r="F2" t="str">
+        <v>Catalina Park</v>
+      </c>
+      <c r="G2" t="str">
         <v>EPL1, Panny20mm</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <v>Peter Sefton</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v>Photo snapped on a photo walk on a misty day</v>
       </c>
     </row>
@@ -948,15 +948,18 @@
         <v>CreateAction</v>
       </c>
       <c r="D3" t="str">
+        <v>2018:09:19T17:01:07+10:00</v>
+      </c>
+      <c r="E3" t="str">
         <v>pics/sepia_fence.jpg</v>
       </c>
-      <c r="E3" t="str">
+      <c r="F3" t="str">
         <v>pics/2017-06-11 12.56.14.jpg</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <v>ImageMagick</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <v>convert -sepia-tone 80% test_data/sample/pics/2017-06-11\ 12.56.14.jpg test_data/sample/pics/sepia_fence.jpg</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made some changes to ID handling and then undid them.
</commit_message>
<xml_diff>
--- a/test_data/sample/CATALOG_sample.xlsx
+++ b/test_data/sample/CATALOG_sample.xlsx
@@ -404,7 +404,7 @@
         <v>Name</v>
       </c>
       <c r="B2" t="str">
-        <v>Sample dataset for DataCrate v0.3</v>
+        <v>Sample dataset for DataCrate v1.0</v>
       </c>
     </row>
     <row r="3">
@@ -719,7 +719,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Equipment"/>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -800,20 +800,6 @@
       </c>
       <c r="H3" t="str">
         <v>Panasonic</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>https://www.imagemagick.org/</v>
-      </c>
-      <c r="B4" t="str">
-        <v>ImageMagick</v>
-      </c>
-      <c r="E4" t="str">
-        <v>https://www.imagemagick.org/</v>
-      </c>
-      <c r="F4" t="str">
-        <v>SoftwareApplicatio n</v>
       </c>
     </row>
   </sheetData>
@@ -959,6 +945,9 @@
       <c r="G3" t="str">
         <v>ImageMagick</v>
       </c>
+      <c r="H3" t="str">
+        <v>Peter Sefton</v>
+      </c>
       <c r="I3" t="str">
         <v>convert -sepia-tone 80% test_data/sample/pics/2017-06-11\ 12.56.14.jpg test_data/sample/pics/sepia_fence.jpg</v>
       </c>

</xml_diff>